<commit_message>
added some colors in  FillColorHex
</commit_message>
<xml_diff>
--- a/src/main/resources/calc/colors.xlsx
+++ b/src/main/resources/calc/colors.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
+  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
   <workbookProtection/>
   <bookViews>
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
@@ -47,12 +47,12 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FFC9211E"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -61,26 +61,56 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF158466"/>
-        <bgColor rgb="FF008080"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00A933"/>
-        <bgColor rgb="FF158466"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF81D41A"/>
-        <bgColor rgb="FFBBE33D"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBBE33D"/>
-        <bgColor rgb="FF81D41A"/>
+        <fgColor rgb="FFFF0000"/>
+        <bgColor rgb="FFF10D0C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFD7D7"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFA6A6"/>
+        <bgColor rgb="FFC0C0C0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF6D6D"/>
+        <bgColor rgb="FFFF3838"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3838"/>
+        <bgColor rgb="FFC9211E"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF10D0C"/>
+        <bgColor rgb="FFFF0000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9211E"/>
+        <bgColor rgb="FFF10D0C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8D281E"/>
+        <bgColor rgb="FF993366"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF50200C"/>
+        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
   </fills>
@@ -118,12 +148,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -139,11 +169,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="10" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -166,20 +208,20 @@
       <rgbColor rgb="FFFFFF00"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
-      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FFF10D0C"/>
       <rgbColor rgb="FF008000"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF158466"/>
+      <rgbColor rgb="FF008080"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
-      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FFFFFFCC"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FF660066"/>
-      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FFFF6D6D"/>
       <rgbColor rgb="FF0066CC"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
@@ -195,22 +237,22 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFA6A6"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFD7D7"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
-      <rgbColor rgb="FF81D41A"/>
-      <rgbColor rgb="FFBBE33D"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF9900"/>
-      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FFFF3838"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF00A933"/>
+      <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FFC9211E"/>
+      <rgbColor rgb="FF50200C"/>
+      <rgbColor rgb="FF8D281E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -224,52 +266,63 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="topLeft" activeCell="D10" activeCellId="0" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
+      <c r="A1" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2"/>
+      <c r="A2" s="2" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="3"/>
+      <c r="A3" s="3" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4"/>
+      <c r="A4" s="4" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="5" t="n">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5"/>
+      <c r="A6" s="6" t="n">
+        <v>6</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7" t="n">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="6"/>
+      <c r="A8" s="8" t="n">
+        <v>8</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6"/>
+      <c r="A9" s="9" t="n">
+        <v>9</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="6"/>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="6"/>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="6"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="6"/>
+      <c r="A10" s="0" t="n">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>